<commit_message>
changes to sample data and pushed alltables into the HappyHealth database using MYSQL
</commit_message>
<xml_diff>
--- a/Design Data/Updated/Sample Data/Sample data for entities.xlsx
+++ b/Design Data/Updated/Sample Data/Sample data for entities.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538106\Desktop\gdp_health_app\Design Data\Sample Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538096\Documents\COURSE\fall 2020\GDP1\gdp_health_app\Design Data\Updated\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4063EA-BEA4-49F4-A2F0-63AAED475EED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="1" r:id="rId1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="165">
   <si>
     <t>UserName</t>
   </si>
@@ -532,7 +531,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -865,23 +864,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection sqref="A1:A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -904,7 +903,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -927,7 +926,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -950,7 +949,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -973,7 +972,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -996,7 +995,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1019,7 +1018,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1042,7 +1041,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1065,7 +1064,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1088,7 +1087,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1111,7 +1110,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1134,7 +1133,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1157,7 +1156,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1180,7 +1179,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1203,7 +1202,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1226,7 +1225,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1249,7 +1248,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1272,7 +1271,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1295,7 +1294,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1318,7 +1317,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1341,7 +1340,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1366,51 +1365,51 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="Robert@123" xr:uid="{3347211E-3829-4382-9239-B9B077165BC5}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{5228730F-885D-47A6-A7E0-A162BDCF5E55}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{B0A50E7C-7C9A-40F4-B015-13BAAA6D5A4E}"/>
-    <hyperlink ref="G3" r:id="rId4" xr:uid="{7CAFCF24-F39C-4702-AEF1-E6B65ADA8339}"/>
-    <hyperlink ref="G5" r:id="rId5" xr:uid="{52564640-A09D-4DD4-AA15-4E1F963A5A96}"/>
-    <hyperlink ref="G6" r:id="rId6" xr:uid="{3D9B5D5C-A1FC-4813-8D10-E70CA7700712}"/>
-    <hyperlink ref="G7" r:id="rId7" xr:uid="{4D04BDB0-949F-44F7-BC69-967026F8AA59}"/>
-    <hyperlink ref="G8" r:id="rId8" xr:uid="{08BB6BF4-8B56-44A8-9301-832D411AB37C}"/>
-    <hyperlink ref="G9" r:id="rId9" xr:uid="{D5E080B8-77D8-4CD3-9FDC-4F1CFD4241B7}"/>
-    <hyperlink ref="G10" r:id="rId10" xr:uid="{053DE528-A767-4B40-A0C0-C703B91041E3}"/>
-    <hyperlink ref="G11" r:id="rId11" xr:uid="{7757F34F-1B79-4337-A599-64B58367EABC}"/>
-    <hyperlink ref="G12" r:id="rId12" xr:uid="{7126E6D9-7084-4FE4-8E48-B08E65A9AD19}"/>
-    <hyperlink ref="G13" r:id="rId13" xr:uid="{7D931926-1307-4412-B48E-C8D98464BC9F}"/>
-    <hyperlink ref="G14" r:id="rId14" xr:uid="{2AF7EAA7-15D0-4B36-8ADD-8C76C2154699}"/>
-    <hyperlink ref="G15" r:id="rId15" xr:uid="{3278AA43-3DDC-498A-B05C-0E895FBD8A2A}"/>
-    <hyperlink ref="G16" r:id="rId16" xr:uid="{EE68A9A4-EA6F-48BB-9B03-3E505BDAA9C6}"/>
-    <hyperlink ref="G17" r:id="rId17" xr:uid="{77B8CE60-7DCB-45A3-8A98-801F7E1A7E3F}"/>
-    <hyperlink ref="G18" r:id="rId18" xr:uid="{B24B901E-893F-4984-A499-B0DFB18E098F}"/>
-    <hyperlink ref="G19" r:id="rId19" xr:uid="{A5CF0B6B-1442-4DD4-B5DB-DC3E4E384C5E}"/>
-    <hyperlink ref="G20" r:id="rId20" xr:uid="{898A5BCA-0599-4270-B807-96AF27726815}"/>
-    <hyperlink ref="G21" r:id="rId21" xr:uid="{C8F1F872-9893-477C-B591-89861B47609D}"/>
+    <hyperlink ref="B4" r:id="rId1" display="Robert@123"/>
+    <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
+    <hyperlink ref="G5" r:id="rId5"/>
+    <hyperlink ref="G6" r:id="rId6"/>
+    <hyperlink ref="G7" r:id="rId7"/>
+    <hyperlink ref="G8" r:id="rId8"/>
+    <hyperlink ref="G9" r:id="rId9"/>
+    <hyperlink ref="G10" r:id="rId10"/>
+    <hyperlink ref="G11" r:id="rId11"/>
+    <hyperlink ref="G12" r:id="rId12"/>
+    <hyperlink ref="G13" r:id="rId13"/>
+    <hyperlink ref="G14" r:id="rId14"/>
+    <hyperlink ref="G15" r:id="rId15"/>
+    <hyperlink ref="G16" r:id="rId16"/>
+    <hyperlink ref="G17" r:id="rId17"/>
+    <hyperlink ref="G18" r:id="rId18"/>
+    <hyperlink ref="G19" r:id="rId19"/>
+    <hyperlink ref="G20" r:id="rId20"/>
+    <hyperlink ref="G21" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8B5DDD-F88B-4D5E-A728-87E46A470DE7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection sqref="A1:F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1430,7 +1429,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1470,7 +1469,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1490,7 +1489,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1510,7 +1509,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1530,7 +1529,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1550,7 +1549,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1570,7 +1569,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1590,7 +1589,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1610,7 +1609,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1630,7 +1629,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1650,7 +1649,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1670,7 +1669,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1690,7 +1689,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1710,7 +1709,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1730,7 +1729,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1750,7 +1749,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1770,7 +1769,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1810,7 +1809,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1837,22 +1836,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB4E68C-0CA9-4C18-8847-54715EEB10BD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
@@ -1866,7 +1865,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1880,7 +1879,7 @@
         <v>0.76113425925925926</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -1894,7 +1893,7 @@
         <v>0.63359953703703698</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -1908,7 +1907,7 @@
         <v>0.67899305555555556</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -1922,7 +1921,7 @@
         <v>0.59625000000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -1936,7 +1935,7 @@
         <v>0.50706018518518514</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -1950,7 +1949,7 @@
         <v>0.42372685185185183</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -1964,7 +1963,7 @@
         <v>0.46609953703703705</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -1978,7 +1977,7 @@
         <v>0.50847222222222221</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>85</v>
       </c>
@@ -1992,7 +1991,7 @@
         <v>0.55084490740740744</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -2006,7 +2005,7 @@
         <v>0.59321759259259255</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -2020,7 +2019,7 @@
         <v>0.63559027777777777</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -2034,7 +2033,7 @@
         <v>0.67868055555555562</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>89</v>
       </c>
@@ -2048,7 +2047,7 @@
         <v>0.72105324074074073</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -2062,7 +2061,7 @@
         <v>0.76342592592592595</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -2076,7 +2075,7 @@
         <v>0.80579861111111117</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>92</v>
       </c>
@@ -2090,7 +2089,7 @@
         <v>0.84817129629629628</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -2104,7 +2103,7 @@
         <v>0.89054398148148151</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>94</v>
       </c>
@@ -2118,7 +2117,7 @@
         <v>0.93291666666666673</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>95</v>
       </c>
@@ -2132,7 +2131,7 @@
         <v>0.9758796296296296</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>96</v>
       </c>
@@ -2153,204 +2152,268 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493B3549-B49E-4EC2-836B-66FF9983BD48}">
-  <dimension ref="A1:D21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3">
         <v>44084</v>
       </c>
-      <c r="B2" s="3">
+      <c r="C2" s="3">
         <v>44085</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3">
         <v>44085</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>44086</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>44087</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3">
         <v>44086</v>
       </c>
-      <c r="B4" s="3">
+      <c r="C4" s="3">
         <v>44088</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3">
         <v>44083</v>
       </c>
-      <c r="B5" s="3">
+      <c r="C5" s="3">
         <v>44084</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3">
         <v>44086</v>
-      </c>
-      <c r="C6" s="3">
-        <v>44088</v>
       </c>
       <c r="D6" s="3">
         <v>44088</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
+      <c r="E6" s="3">
         <v>44088</v>
       </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
       <c r="B7" s="3">
+        <v>44088</v>
+      </c>
+      <c r="C7" s="3">
         <v>44090</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3">
         <v>44082</v>
       </c>
-      <c r="B8" s="3">
+      <c r="C8" s="3">
         <v>44084</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3">
         <v>44083</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="3">
         <v>44084</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3">
         <v>44084</v>
       </c>
-      <c r="B10" s="3">
+      <c r="C10" s="3">
         <v>44085</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3">
         <v>44085</v>
       </c>
-      <c r="C11" s="3">
+      <c r="D11" s="3">
         <v>44087</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="3">
         <v>44086</v>
       </c>
-      <c r="B12" s="3">
+      <c r="C12" s="3">
         <v>44089</v>
       </c>
-      <c r="D12" s="3">
+      <c r="E12" s="3">
         <v>44094</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3">
         <v>44087</v>
       </c>
-      <c r="B13" s="3">
+      <c r="C13" s="3">
         <v>44091</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
-        <v>44089</v>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
       </c>
       <c r="B14" s="3">
         <v>44089</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
-        <v>44083</v>
+      <c r="C14" s="3">
+        <v>44089</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
       </c>
       <c r="B15" s="3">
         <v>44083</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
-        <v>44085</v>
+      <c r="C15" s="3">
+        <v>44083</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
       </c>
       <c r="B16" s="3">
         <v>44085</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
+      <c r="C16" s="3">
+        <v>44085</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3">
         <v>44084</v>
       </c>
-      <c r="C17" s="3">
+      <c r="D17" s="3">
         <v>44084</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="3">
         <v>44086</v>
       </c>
-      <c r="B18" s="3">
+      <c r="C18" s="3">
         <v>44087</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="3">
         <v>44086</v>
       </c>
-      <c r="C19" s="3">
+      <c r="D19" s="3">
         <v>44087</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
-        <v>44084</v>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
       </c>
       <c r="B20" s="3">
         <v>44084</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="3">
+      <c r="C20" s="3">
+        <v>44084</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="3">
         <v>44082</v>
       </c>
-      <c r="B21" s="3">
+      <c r="C21" s="3">
         <v>44083</v>
       </c>
     </row>
@@ -2361,21 +2424,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3FC752-2CCC-4ADA-BD93-3CC74B8D634B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection sqref="A1:D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2389,7 +2452,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -2400,7 +2463,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>50</v>
       </c>
@@ -2414,7 +2477,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -2426,7 +2489,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>52</v>
       </c>
@@ -2437,7 +2500,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>53</v>
       </c>
@@ -2448,7 +2511,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>54</v>
       </c>
@@ -2459,7 +2522,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>55</v>
       </c>
@@ -2470,7 +2533,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
@@ -2481,7 +2544,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>57</v>
       </c>
@@ -2492,7 +2555,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>58</v>
       </c>
@@ -2503,7 +2566,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>59</v>
       </c>
@@ -2517,7 +2580,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>60</v>
       </c>
@@ -2528,7 +2591,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>61</v>
       </c>
@@ -2539,7 +2602,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
@@ -2550,7 +2613,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>63</v>
       </c>
@@ -2561,7 +2624,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>64</v>
       </c>
@@ -2572,7 +2635,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>65</v>
       </c>
@@ -2583,7 +2646,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>66</v>
       </c>
@@ -2594,7 +2657,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>67</v>
       </c>
@@ -2605,7 +2668,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>68</v>
       </c>
@@ -2621,49 +2684,49 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{3E500F6C-B005-4FD5-8341-0D4C4A577D27}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{BFB5CEBE-6EB3-4570-8965-2DCB8FB32D38}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{9EAAF5F8-91C6-4EF4-9859-4BF770C9F797}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{646DD1EC-D6F8-4A8F-87C9-A2B06877C90B}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{55B87998-C303-4D7D-BEAF-25AE81CF0C4B}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{CB1055F4-3CEB-4A08-B4E6-1E69BAA61ACA}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{D47F77C1-1A5C-45A4-B98C-D619872E4FBF}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{6B0A71EC-7E8F-4C35-94CE-98F93A7328FA}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{965153E3-7822-4672-9FA9-5ECB188BCE68}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{671C8B7F-CE8C-44B6-8639-C8DA1E203EF5}"/>
-    <hyperlink ref="A12" r:id="rId11" xr:uid="{DCF8ED35-D9DD-4723-B47B-76E692EE915C}"/>
-    <hyperlink ref="A13" r:id="rId12" xr:uid="{895E4CA8-8A92-4A57-86DF-EEBFADF626D0}"/>
-    <hyperlink ref="A14" r:id="rId13" xr:uid="{69A3ABD1-BD14-45DA-A50D-D10F01D0F840}"/>
-    <hyperlink ref="A15" r:id="rId14" xr:uid="{B2A18679-5418-45E7-BDDC-39DA803A3AE1}"/>
-    <hyperlink ref="A16" r:id="rId15" xr:uid="{68833912-76FC-489C-81B9-A4CA3F3FBD65}"/>
-    <hyperlink ref="A17" r:id="rId16" xr:uid="{BE93573C-0BF2-437C-9D44-3397269A53B8}"/>
-    <hyperlink ref="A18" r:id="rId17" xr:uid="{E2ECD02D-96EC-439D-8E28-7832B9CBED1B}"/>
-    <hyperlink ref="A19" r:id="rId18" xr:uid="{4F6E11E7-5BE1-47CB-BD9F-4B36DEA13662}"/>
-    <hyperlink ref="A20" r:id="rId19" xr:uid="{F93FA330-E38A-4B94-8646-F15A6B2D8B55}"/>
-    <hyperlink ref="A21" r:id="rId20" xr:uid="{84BFF350-6702-4C0F-84D4-9F8DBD1DE976}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A13" r:id="rId12"/>
+    <hyperlink ref="A14" r:id="rId13"/>
+    <hyperlink ref="A15" r:id="rId14"/>
+    <hyperlink ref="A16" r:id="rId15"/>
+    <hyperlink ref="A17" r:id="rId16"/>
+    <hyperlink ref="A18" r:id="rId17"/>
+    <hyperlink ref="A19" r:id="rId18"/>
+    <hyperlink ref="A20" r:id="rId19"/>
+    <hyperlink ref="A21" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BCB583-04A0-41CC-9CF1-170A1216D898}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F21"/>
+      <selection sqref="A1:H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>108</v>
       </c>
@@ -2689,7 +2752,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2715,7 +2778,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2741,7 +2804,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2767,7 +2830,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2793,7 +2856,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2819,7 +2882,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2845,7 +2908,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2871,7 +2934,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2897,7 +2960,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2923,7 +2986,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2949,7 +3012,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2975,7 +3038,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -3001,7 +3064,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -3027,7 +3090,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -3053,7 +3116,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -3079,7 +3142,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -3105,7 +3168,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -3131,7 +3194,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -3157,7 +3220,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -3183,7 +3246,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -3216,22 +3279,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416BFC41-9C5D-43DC-823F-34B7584A6B33}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E21"/>
+      <selection sqref="A1:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>112</v>
       </c>
@@ -3248,7 +3311,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1091</v>
       </c>
@@ -3265,9 +3328,9 @@
         <v>0.50706018518518514</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="B3" t="s">
         <v>149</v>
@@ -3282,9 +3345,9 @@
         <v>0.42372685185185183</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="B4" t="s">
         <v>150</v>
@@ -3299,9 +3362,9 @@
         <v>0.46609953703703705</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="B5" t="s">
         <v>151</v>
@@ -3316,9 +3379,9 @@
         <v>0.50847222222222221</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="B6" t="s">
         <v>152</v>
@@ -3333,9 +3396,9 @@
         <v>0.55084490740740744</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B7" t="s">
         <v>153</v>
@@ -3350,9 +3413,9 @@
         <v>0.59321759259259255</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="B8" t="s">
         <v>154</v>
@@ -3367,9 +3430,9 @@
         <v>0.63559027777777777</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="B9" t="s">
         <v>155</v>
@@ -3384,9 +3447,9 @@
         <v>0.67868055555555562</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="B10" t="s">
         <v>156</v>
@@ -3401,194 +3464,51 @@
         <v>0.72105324074074073</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>1099</v>
-      </c>
-      <c r="B11" t="s">
-        <v>148</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="3">
-        <v>44096</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0.76342592592592595</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>1100</v>
-      </c>
-      <c r="B12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="3">
-        <v>44094</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0.80579861111111117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>1081</v>
-      </c>
-      <c r="B13" t="s">
-        <v>150</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="3">
-        <v>44095</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0.84817129629629628</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>1082</v>
-      </c>
-      <c r="B14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="3">
-        <v>44097</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0.89054398148148151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>1083</v>
-      </c>
-      <c r="B15" t="s">
-        <v>152</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="3">
-        <v>44098</v>
-      </c>
-      <c r="E15" s="4">
-        <v>0.93291666666666673</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>1084</v>
-      </c>
-      <c r="B16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="3">
-        <v>44094</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0.9758796296296296</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>1085</v>
-      </c>
-      <c r="B17" t="s">
-        <v>154</v>
-      </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="3">
-        <v>44094</v>
-      </c>
-      <c r="E17" s="4">
-        <v>0.6793865740740741</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>1086</v>
-      </c>
-      <c r="B18" t="s">
-        <v>155</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="3">
-        <v>44094</v>
-      </c>
-      <c r="E18" s="4">
-        <v>0.46609953703703705</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>1087</v>
-      </c>
-      <c r="B19" t="s">
-        <v>156</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="3">
-        <v>44095</v>
-      </c>
-      <c r="E19" s="4">
-        <v>0.50847222222222221</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>1089</v>
-      </c>
-      <c r="B20" t="s">
-        <v>148</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="3">
-        <v>44095</v>
-      </c>
-      <c r="E20" s="4">
-        <v>0.55084490740740744</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>1090</v>
-      </c>
-      <c r="B21" t="s">
-        <v>149</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="3">
-        <v>44096</v>
-      </c>
-      <c r="E21" s="4">
-        <v>0.59321759259259255</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="3"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="3"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E22" s="4"/>
     </row>
   </sheetData>
@@ -3598,22 +3518,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C9F54AA-FF8F-4D91-92A7-2BA1F073E2C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>157</v>
       </c>
@@ -3627,7 +3547,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>158</v>
       </c>
@@ -3641,7 +3561,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>159</v>
       </c>
@@ -3655,7 +3575,7 @@
         <v>0.49733796296296301</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>160</v>
       </c>
@@ -3669,7 +3589,7 @@
         <v>0.42443287037037036</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -3683,7 +3603,7 @@
         <v>0.50847222222222221</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>162</v>
       </c>
@@ -3697,7 +3617,7 @@
         <v>0.55084490740740744</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>163</v>
       </c>
@@ -3711,201 +3631,61 @@
         <v>0.63488425925925929</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="3">
-        <v>44097</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.63559027777777777</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3">
-        <v>44096</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.67868055555555562</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>160</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="3">
-        <v>44094</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.72105324074074073</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>161</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="3">
-        <v>44096</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.76342592592592595</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>162</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3">
-        <v>44095</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0.80579861111111117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>163</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="3">
-        <v>44096</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.84817129629629628</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>160</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="3">
-        <v>44097</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.89054398148148151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>159</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="3">
-        <v>44098</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.93291666666666673</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>162</v>
-      </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="3">
-        <v>44095</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0.9758796296296296</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>163</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="3">
-        <v>44094</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0.6793865740740741</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>161</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="3">
-        <v>44096</v>
-      </c>
-      <c r="D18" s="4">
-        <v>0.46609953703703705</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>158</v>
-      </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="3">
-        <v>44094</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0.50847222222222221</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>160</v>
-      </c>
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="3">
-        <v>44095</v>
-      </c>
-      <c r="D20" s="4">
-        <v>0.55084490740740744</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>159</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="3">
-        <v>44097</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0.59321759259259255</v>
-      </c>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>